<commit_message>
Added CLI Support (Clamshell) Split Lambda into 4 sub-modules (Core, CLI, Assembly, Splash) Support for Windows\Linux command-line Paramaterized Lambda runner for use in multiple-interfaces
</commit_message>
<xml_diff>
--- a/lambda-core/src/main/java/au/com/onegeek/lambda/tests/tests-aes.xlsx
+++ b/lambda-core/src/main/java/au/com/onegeek/lambda/tests/tests-aes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="suite-demo1" sheetId="3" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>assertTextPresent</t>
   </si>
   <si>
-    <t>waitForPageToLoad</t>
-  </si>
-  <si>
     <t>thisisadomainname.com.au</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>foobarbaz.com.au</t>
   </si>
   <si>
-    <t>Function</t>
-  </si>
-  <si>
     <t>Target</t>
   </si>
   <si>
@@ -132,6 +126,12 @@
   </si>
   <si>
     <t>maintenance</t>
+  </si>
+  <si>
+    <t>Keyward</t>
+  </si>
+  <si>
+    <t>sleep</t>
   </si>
 </sst>
 </file>
@@ -195,7 +195,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -210,6 +210,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
@@ -230,7 +232,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -239,12 +241,14 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -576,7 +580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -591,13 +597,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -610,10 +616,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -621,26 +627,26 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>36</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5000</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -648,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -676,7 +682,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -703,15 +709,15 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -719,47 +725,46 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -772,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -800,58 +805,58 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>